<commit_message>
Load find_head_tail function correctly and add a package to environment.yml
Former-commit-id: 46e571f773dcafd864855063f74dc3611e2de165
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DM209 |-| DM206</t>
+          <t>DM206 -&gt; DM209</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DM223 |-| DM209</t>
+          <t>DM209 -&gt; DM223</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DM203 |-| DM205</t>
+          <t>DM203 -&gt; DM205</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DM205 |-| DM207</t>
+          <t>DM205 -&gt; DM207</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Glycolaldehyde |-| Glycolate</t>
+          <t>Glycolaldehyde -&gt; Glycolate</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Glyoxylate |-| Hyi</t>
+          <t>Glyoxylate -&gt; tGcl Tartronate semialdehyde</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hydroxypyruvate |-| Glycerate</t>
+          <t>Hydroxypyruvate -&gt; Glycerate</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -791,12 +791,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hydroxypyruvate |-| tGcl Tartronate semialdehyde</t>
+          <t>tGcl Tartronate semialdehyde -&gt; Hydroxypyruvate</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Hyi']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,4-Butanediol |-| 4-Hydroxy-3-Keto-Butyryl-CoA</t>
+          <t>1,4-Butanediol -&gt; 4-Hydroxy-3-Keto-Butyryl-CoA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Glycolate |-| Glyoxylate</t>
+          <t>Glycolate -&gt; Glyoxylate</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Glycolyl-CoA |-| Glycolaldehyde</t>
+          <t>Glycolyl-CoA -&gt; Glycolaldehyde</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Glyoxylate |-| TCA cycle</t>
+          <t>Glyoxylate -&gt; TCA cycle</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Acetyl-CoA |-| TCA cycle</t>
+          <t>Acetyl-CoA -&gt; TCA cycle</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -985,6 +985,41 @@
         </is>
       </c>
       <c r="G16" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PMC10269461_spectrum.04988-22-f004.jpg</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GCLpathway -&gt; Acetyl-CoA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>